<commit_message>
Remove CTI and DWI input, update the format and set default parameters to analyse test_data
</commit_message>
<xml_diff>
--- a/template_files/template_parameters_analysis.xlsx
+++ b/template_files/template_parameters_analysis.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10514"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10719"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/u0112736/Documents/MATLAB/NET_v2.24/template_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B56BFCB-0800-AA41-BC4E-B18A3D5E102D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F62A9E8-E818-D248-BDE6-FD34796FEFE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1060" yWindow="500" windowWidth="20180" windowHeight="16100" activeTab="2" xr2:uid="{6EC9E106-9E35-B247-8D86-0F73FA459190}"/>
+    <workbookView xWindow="10060" yWindow="760" windowWidth="20180" windowHeight="16100" activeTab="2" xr2:uid="{6EC9E106-9E35-B247-8D86-0F73FA459190}"/>
   </bookViews>
   <sheets>
     <sheet name="activity_analysis" sheetId="1" r:id="rId1"/>
@@ -739,7 +739,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="8">
+  <dxfs count="14">
     <dxf>
       <font>
         <b/>
@@ -752,6 +752,20 @@
         <b/>
         <i val="0"/>
         <color rgb="FFED7D31"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF00B050"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFFF0000"/>
       </font>
     </dxf>
     <dxf>
@@ -786,6 +800,20 @@
       <font>
         <b/>
         <i val="0"/>
+        <color rgb="FF00B050"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
         <color theme="6" tint="-0.24994659260841701"/>
       </font>
     </dxf>
@@ -794,6 +822,20 @@
         <b/>
         <i val="0"/>
         <color rgb="FFED7D31"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF00B050"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFFF0000"/>
       </font>
     </dxf>
   </dxfs>
@@ -1116,7 +1158,7 @@
   <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1143,7 +1185,7 @@
         <v>3</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>5</v>
@@ -1220,7 +1262,7 @@
         <v>19</v>
       </c>
       <c r="B9" s="19" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="C9" s="20" t="s">
         <v>5</v>
@@ -1231,7 +1273,7 @@
         <v>20</v>
       </c>
       <c r="B10" s="19" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="C10" s="20" t="s">
         <v>5</v>
@@ -1253,7 +1295,7 @@
         <v>23</v>
       </c>
       <c r="B12" s="19" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="C12" s="20" t="s">
         <v>5</v>
@@ -1294,10 +1336,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B1:B1048576">
-    <cfRule type="cellIs" dxfId="7" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="1" operator="equal">
       <formula>"off"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="2" operator="equal">
       <formula>"on"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1310,7 +1352,7 @@
   <dimension ref="A1:C20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1337,7 +1379,7 @@
         <v>28</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>5</v>
@@ -1542,20 +1584,12 @@
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B2:B10 B12:B20">
-    <cfRule type="beginsWith" dxfId="5" priority="3" operator="beginsWith" text="off">
-      <formula>LEFT(B2,LEN("off"))="off"</formula>
+  <conditionalFormatting sqref="B1:B1048576">
+    <cfRule type="beginsWith" dxfId="9" priority="1" operator="beginsWith" text="off">
+      <formula>LEFT(B1,LEN("off"))="off"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="4" priority="4" operator="beginsWith" text="on">
-      <formula>LEFT(B2,LEN("on"))="on"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B11">
-    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
-      <formula>"off"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
-      <formula>"on"</formula>
+    <cfRule type="beginsWith" dxfId="8" priority="2" operator="beginsWith" text="on">
+      <formula>LEFT(B1,LEN("on"))="on"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1567,7 +1601,7 @@
   <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="25" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1615,7 +1649,7 @@
         <v>66</v>
       </c>
       <c r="B4" s="42" t="s">
-        <v>67</v>
+        <v>74</v>
       </c>
       <c r="C4" s="42" t="s">
         <v>68</v>
@@ -1710,12 +1744,12 @@
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B2:B12">
-    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="no">
-      <formula>NOT(ISERROR(SEARCH("no",B2)))</formula>
+  <conditionalFormatting sqref="B1:B1048576">
+    <cfRule type="containsText" dxfId="3" priority="1" operator="containsText" text="no">
+      <formula>NOT(ISERROR(SEARCH("no",B1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="0" priority="2" operator="containsText" text="yes">
-      <formula>NOT(ISERROR(SEARCH("yes",B2)))</formula>
+    <cfRule type="containsText" dxfId="2" priority="2" operator="containsText" text="yes">
+      <formula>NOT(ISERROR(SEARCH("yes",B1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
replace template_no_gui.xls with 3 xls from gui and read correct number of subjs for statistic analysis
</commit_message>
<xml_diff>
--- a/template_files/template_parameters_analysis.xlsx
+++ b/template_files/template_parameters_analysis.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10719"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/u0112736/Documents/MATLAB/NET_v2.24/template_files/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/u0112736/Documents/MATLAB/net/template_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F62A9E8-E818-D248-BDE6-FD34796FEFE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00613AA6-8E46-6849-A1E4-9A927CB003AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10060" yWindow="760" windowWidth="20180" windowHeight="16100" activeTab="2" xr2:uid="{6EC9E106-9E35-B247-8D86-0F73FA459190}"/>
+    <workbookView xWindow="10060" yWindow="760" windowWidth="20180" windowHeight="16100" activeTab="1" xr2:uid="{6EC9E106-9E35-B247-8D86-0F73FA459190}"/>
   </bookViews>
   <sheets>
     <sheet name="activity_analysis" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="88">
   <si>
     <t>parameters_name</t>
   </si>
@@ -67,9 +67,6 @@
     <t>erp.seed_file</t>
   </si>
   <si>
-    <t>seed_testing</t>
-  </si>
-  <si>
     <t>Name of seeds file (template &gt; seeds)</t>
   </si>
   <si>
@@ -91,9 +88,6 @@
     <t>erp.triggers</t>
   </si>
   <si>
-    <t>auditory_oddball_triggers</t>
-  </si>
-  <si>
     <t>Name of trigger file (template &gt; triggers)</t>
   </si>
   <si>
@@ -106,9 +100,6 @@
     <t>ers_erd.seed_file</t>
   </si>
   <si>
-    <t>seed_ERD_ERS</t>
-  </si>
-  <si>
     <t>ers_erd.mapping_enable</t>
   </si>
   <si>
@@ -119,9 +110,6 @@
   </si>
   <si>
     <t>ers_erd.triggers</t>
-  </si>
-  <si>
-    <t>gait_ERD_ERS_triggers</t>
   </si>
   <si>
     <t>ica_conn.enable</t>
@@ -247,9 +235,6 @@
     <t>seeding.seed_file</t>
   </si>
   <si>
-    <t>seeds_DePasquale</t>
-  </si>
-  <si>
     <t>stats.flag</t>
   </si>
   <si>
@@ -338,6 +323,12 @@
   </si>
   <si>
     <t>Prefix of MNI individual maps: I) activity analysis (''erp'',''ers_erd''); II) connectivity analysis (''rsn'',''seed'')</t>
+  </si>
+  <si>
+    <t>template_seeds</t>
+  </si>
+  <si>
+    <t>template_10_July</t>
   </si>
 </sst>
 </file>
@@ -601,7 +592,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -629,9 +620,6 @@
     </xf>
     <xf numFmtId="49" fontId="2" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -739,19 +727,19 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="14">
+  <dxfs count="10">
     <dxf>
       <font>
         <b/>
         <i val="0"/>
-        <color rgb="FF808080"/>
+        <color rgb="FF00B050"/>
       </font>
     </dxf>
     <dxf>
       <font>
         <b/>
         <i val="0"/>
-        <color rgb="FFED7D31"/>
+        <color rgb="FFFF0000"/>
       </font>
     </dxf>
     <dxf>
@@ -772,28 +760,14 @@
       <font>
         <b/>
         <i val="0"/>
-        <color theme="6" tint="-0.24994659260841701"/>
+        <color rgb="FF00B050"/>
       </font>
     </dxf>
     <dxf>
       <font>
         <b/>
         <i val="0"/>
-        <color rgb="FFED7D31"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="0" tint="-0.499984740745262"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFED7D31"/>
+        <color rgb="FFFF0000"/>
       </font>
     </dxf>
     <dxf>
@@ -808,20 +782,6 @@
         <b/>
         <i val="0"/>
         <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="6" tint="-0.24994659260841701"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFED7D31"/>
       </font>
     </dxf>
     <dxf>
@@ -1158,7 +1118,7 @@
   <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1206,16 +1166,16 @@
       <c r="A4" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="10" t="s">
+      <c r="B4" s="15" t="s">
+        <v>86</v>
+      </c>
+      <c r="C4" s="10" t="s">
         <v>9</v>
-      </c>
-      <c r="C4" s="11" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="18" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B5" s="7" t="s">
         <v>7</v>
@@ -1225,122 +1185,130 @@
       </c>
     </row>
     <row r="6" spans="1:3" ht="18" x14ac:dyDescent="0.2">
-      <c r="A6" s="12" t="s">
+      <c r="A6" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="12">
+        <v>1</v>
+      </c>
+      <c r="C6" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="13">
+    </row>
+    <row r="7" spans="1:3" ht="18" x14ac:dyDescent="0.2">
+      <c r="A7" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" s="12">
+        <v>80</v>
+      </c>
+      <c r="C7" s="13" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="19" x14ac:dyDescent="0.2">
+      <c r="A8" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" s="15" t="s">
+        <v>87</v>
+      </c>
+      <c r="C8" s="16" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="18" x14ac:dyDescent="0.2">
+      <c r="A9" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" s="19" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="18" x14ac:dyDescent="0.2">
+      <c r="A10" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10" s="19" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="19" x14ac:dyDescent="0.2">
+      <c r="A11" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="B11" s="34" t="s">
+        <v>86</v>
+      </c>
+      <c r="C11" s="22" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="18" x14ac:dyDescent="0.2">
+      <c r="A12" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="B12" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="C12" s="19" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="18" x14ac:dyDescent="0.2">
+      <c r="A13" s="23" t="s">
+        <v>21</v>
+      </c>
+      <c r="B13" s="24">
         <v>1</v>
       </c>
-      <c r="C6" s="14" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="18" x14ac:dyDescent="0.2">
-      <c r="A7" s="12" t="s">
+      <c r="C13" s="25" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="18" x14ac:dyDescent="0.2">
+      <c r="A14" s="23" t="s">
+        <v>22</v>
+      </c>
+      <c r="B14" s="24">
+        <v>80</v>
+      </c>
+      <c r="C14" s="25" t="s">
         <v>14</v>
       </c>
-      <c r="B7" s="13">
-        <v>80</v>
-      </c>
-      <c r="C7" s="14" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" ht="19" x14ac:dyDescent="0.2">
-      <c r="A8" s="15" t="s">
+    </row>
+    <row r="15" spans="1:3" ht="19" x14ac:dyDescent="0.2">
+      <c r="A15" s="26" t="s">
+        <v>23</v>
+      </c>
+      <c r="B15" s="27" t="s">
+        <v>87</v>
+      </c>
+      <c r="C15" s="28" t="s">
         <v>16</v>
       </c>
-      <c r="B8" s="16" t="s">
-        <v>17</v>
-      </c>
-      <c r="C8" s="17" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" ht="18" x14ac:dyDescent="0.2">
-      <c r="A9" s="18" t="s">
-        <v>19</v>
-      </c>
-      <c r="B9" s="19" t="s">
-        <v>7</v>
-      </c>
-      <c r="C9" s="20" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" ht="18" x14ac:dyDescent="0.2">
-      <c r="A10" s="18" t="s">
-        <v>20</v>
-      </c>
-      <c r="B10" s="19" t="s">
-        <v>7</v>
-      </c>
-      <c r="C10" s="20" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" ht="19" x14ac:dyDescent="0.2">
-      <c r="A11" s="21" t="s">
-        <v>21</v>
-      </c>
-      <c r="B11" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="C11" s="23" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" ht="18" x14ac:dyDescent="0.2">
-      <c r="A12" s="18" t="s">
-        <v>23</v>
-      </c>
-      <c r="B12" s="19" t="s">
-        <v>7</v>
-      </c>
-      <c r="C12" s="20" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" ht="18" x14ac:dyDescent="0.2">
-      <c r="A13" s="24" t="s">
-        <v>24</v>
-      </c>
-      <c r="B13" s="25">
-        <v>1</v>
-      </c>
-      <c r="C13" s="26" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" ht="18" x14ac:dyDescent="0.2">
-      <c r="A14" s="24" t="s">
-        <v>25</v>
-      </c>
-      <c r="B14" s="25">
-        <v>80</v>
-      </c>
-      <c r="C14" s="26" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" ht="19" x14ac:dyDescent="0.2">
-      <c r="A15" s="27" t="s">
-        <v>26</v>
-      </c>
-      <c r="B15" s="28" t="s">
-        <v>27</v>
-      </c>
-      <c r="C15" s="29" t="s">
-        <v>18</v>
-      </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B1:B1048576">
-    <cfRule type="cellIs" dxfId="13" priority="1" operator="equal">
+  <conditionalFormatting sqref="B12:B1048576 B1:B10">
+    <cfRule type="cellIs" dxfId="9" priority="5" operator="equal">
       <formula>"off"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="6" operator="equal">
       <formula>"on"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B11">
+    <cfRule type="beginsWith" dxfId="3" priority="3" operator="beginsWith" text="off">
+      <formula>LEFT(B11,LEN("off"))="off"</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="2" priority="4" operator="beginsWith" text="on">
+      <formula>LEFT(B11,LEN("on"))="on"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1351,8 +1319,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B89B74C7-BC73-5F44-99BC-879A3B054F87}">
   <dimension ref="A1:C20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1364,19 +1332,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="18" x14ac:dyDescent="0.2">
-      <c r="A1" s="30" t="s">
+      <c r="A1" s="29" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="31" t="s">
+      <c r="C1" s="30" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="18" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>4</v>
@@ -1386,209 +1354,209 @@
       </c>
     </row>
     <row r="3" spans="1:3" ht="18" x14ac:dyDescent="0.2">
-      <c r="A3" s="12" t="s">
+      <c r="A3" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="B3" s="12">
+        <v>1</v>
+      </c>
+      <c r="C3" s="13" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="18" x14ac:dyDescent="0.2">
+      <c r="A4" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="B4" s="12">
+        <v>80</v>
+      </c>
+      <c r="C4" s="13" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="18" x14ac:dyDescent="0.2">
+      <c r="A5" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="B5" s="12">
+        <v>2</v>
+      </c>
+      <c r="C5" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="B3" s="13">
+    </row>
+    <row r="6" spans="1:3" ht="18" x14ac:dyDescent="0.2">
+      <c r="A6" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="B6" s="12">
         <v>1</v>
       </c>
-      <c r="C3" s="14" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="18" x14ac:dyDescent="0.2">
-      <c r="A4" s="12" t="s">
-        <v>30</v>
-      </c>
-      <c r="B4" s="13">
-        <v>80</v>
-      </c>
-      <c r="C4" s="14" t="s">
+      <c r="C6" s="13" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="18" x14ac:dyDescent="0.2">
-      <c r="A5" s="12" t="s">
+    <row r="7" spans="1:3" ht="18" x14ac:dyDescent="0.2">
+      <c r="A7" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="B5" s="13">
+      <c r="B7" s="12">
+        <v>6</v>
+      </c>
+      <c r="C7" s="13" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="18" x14ac:dyDescent="0.2">
+      <c r="A8" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="B8" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="C8" s="13" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="18" x14ac:dyDescent="0.2">
+      <c r="A9" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="B9" s="31" t="s">
+        <v>38</v>
+      </c>
+      <c r="C9" s="13" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="18" x14ac:dyDescent="0.2">
+      <c r="A10" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="B10" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="C10" s="13" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="19" x14ac:dyDescent="0.2">
+      <c r="A11" s="11" t="s">
+        <v>82</v>
+      </c>
+      <c r="B11" s="15" t="s">
+        <v>87</v>
+      </c>
+      <c r="C11" s="16" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="18" x14ac:dyDescent="0.2">
+      <c r="A12" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="B12" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="C12" s="19" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="18" x14ac:dyDescent="0.2">
+      <c r="A13" s="17" t="s">
+        <v>44</v>
+      </c>
+      <c r="B13" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="C13" s="19" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="18" x14ac:dyDescent="0.2">
+      <c r="A14" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="B14" s="32">
         <v>2</v>
       </c>
-      <c r="C5" s="14" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="18" x14ac:dyDescent="0.2">
-      <c r="A6" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="B6" s="13">
+      <c r="C14" s="25" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="18" x14ac:dyDescent="0.2">
+      <c r="A15" s="23" t="s">
+        <v>46</v>
+      </c>
+      <c r="B15" s="32">
         <v>1</v>
       </c>
-      <c r="C6" s="14" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="18" x14ac:dyDescent="0.2">
-      <c r="A7" s="12" t="s">
-        <v>36</v>
-      </c>
-      <c r="B7" s="13">
-        <v>6</v>
-      </c>
-      <c r="C7" s="14" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" ht="18" x14ac:dyDescent="0.2">
-      <c r="A8" s="12" t="s">
-        <v>38</v>
-      </c>
-      <c r="B8" s="13" t="s">
-        <v>39</v>
-      </c>
-      <c r="C8" s="14" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" ht="18" x14ac:dyDescent="0.2">
-      <c r="A9" s="12" t="s">
-        <v>41</v>
-      </c>
-      <c r="B9" s="32" t="s">
-        <v>42</v>
-      </c>
-      <c r="C9" s="14" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" ht="18" x14ac:dyDescent="0.2">
-      <c r="A10" s="12" t="s">
-        <v>44</v>
-      </c>
-      <c r="B10" s="13" t="s">
-        <v>45</v>
-      </c>
-      <c r="C10" s="14" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" ht="19" x14ac:dyDescent="0.2">
-      <c r="A11" s="12" t="s">
+      <c r="C15" s="25" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="19" x14ac:dyDescent="0.2">
+      <c r="A16" s="20" t="s">
+        <v>47</v>
+      </c>
+      <c r="B16" s="21" t="s">
+        <v>48</v>
+      </c>
+      <c r="C16" s="33" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="19" x14ac:dyDescent="0.2">
+      <c r="A17" s="20" t="s">
+        <v>50</v>
+      </c>
+      <c r="B17" s="21" t="s">
+        <v>51</v>
+      </c>
+      <c r="C17" s="22" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="19" x14ac:dyDescent="0.2">
+      <c r="A18" s="20" t="s">
+        <v>53</v>
+      </c>
+      <c r="B18" s="34">
+        <v>1000</v>
+      </c>
+      <c r="C18" s="22" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="19" x14ac:dyDescent="0.2">
+      <c r="A19" s="20" t="s">
+        <v>55</v>
+      </c>
+      <c r="B19" s="34" t="s">
+        <v>86</v>
+      </c>
+      <c r="C19" s="22" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="19" x14ac:dyDescent="0.2">
+      <c r="A20" s="35" t="s">
+        <v>83</v>
+      </c>
+      <c r="B20" s="36" t="s">
         <v>87</v>
       </c>
-      <c r="B11" s="16" t="s">
-        <v>17</v>
-      </c>
-      <c r="C11" s="17" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" ht="18" x14ac:dyDescent="0.2">
-      <c r="A12" s="18" t="s">
-        <v>47</v>
-      </c>
-      <c r="B12" s="19" t="s">
-        <v>4</v>
-      </c>
-      <c r="C12" s="20" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" ht="18" x14ac:dyDescent="0.2">
-      <c r="A13" s="18" t="s">
-        <v>48</v>
-      </c>
-      <c r="B13" s="19" t="s">
-        <v>4</v>
-      </c>
-      <c r="C13" s="20" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" ht="18" x14ac:dyDescent="0.2">
-      <c r="A14" s="24" t="s">
-        <v>49</v>
-      </c>
-      <c r="B14" s="33">
-        <v>2</v>
-      </c>
-      <c r="C14" s="26" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" ht="18" x14ac:dyDescent="0.2">
-      <c r="A15" s="24" t="s">
-        <v>50</v>
-      </c>
-      <c r="B15" s="33">
-        <v>1</v>
-      </c>
-      <c r="C15" s="26" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" ht="19" x14ac:dyDescent="0.2">
-      <c r="A16" s="21" t="s">
-        <v>51</v>
-      </c>
-      <c r="B16" s="22" t="s">
-        <v>52</v>
-      </c>
-      <c r="C16" s="34" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" ht="19" x14ac:dyDescent="0.2">
-      <c r="A17" s="21" t="s">
-        <v>54</v>
-      </c>
-      <c r="B17" s="22" t="s">
-        <v>55</v>
-      </c>
-      <c r="C17" s="23" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" ht="19" x14ac:dyDescent="0.2">
-      <c r="A18" s="21" t="s">
-        <v>57</v>
-      </c>
-      <c r="B18" s="35">
-        <v>1000</v>
-      </c>
-      <c r="C18" s="23" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" ht="19" x14ac:dyDescent="0.2">
-      <c r="A19" s="21" t="s">
-        <v>59</v>
-      </c>
-      <c r="B19" s="35" t="s">
-        <v>60</v>
-      </c>
-      <c r="C19" s="23" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" ht="19" x14ac:dyDescent="0.2">
-      <c r="A20" s="36" t="s">
-        <v>88</v>
-      </c>
-      <c r="B20" s="37" t="s">
-        <v>17</v>
-      </c>
-      <c r="C20" s="38" t="s">
-        <v>89</v>
+      <c r="C20" s="37" t="s">
+        <v>84</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="B1:B1048576">
-    <cfRule type="beginsWith" dxfId="9" priority="1" operator="beginsWith" text="off">
+    <cfRule type="beginsWith" dxfId="7" priority="1" operator="beginsWith" text="off">
       <formula>LEFT(B1,LEN("off"))="off"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="8" priority="2" operator="beginsWith" text="on">
+    <cfRule type="beginsWith" dxfId="6" priority="2" operator="beginsWith" text="on">
       <formula>LEFT(B1,LEN("on"))="on"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1600,7 +1568,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A225D7CE-8777-D54B-A402-94CEC95943B4}">
   <dimension ref="A1:C12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
@@ -1612,143 +1580,143 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="18" x14ac:dyDescent="0.2">
-      <c r="A1" s="39" t="s">
+      <c r="A1" s="38" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="39" t="s">
+      <c r="B1" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="39" t="s">
+      <c r="C1" s="38" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="18" x14ac:dyDescent="0.2">
-      <c r="A2" s="40" t="s">
+      <c r="A2" s="39" t="s">
+        <v>56</v>
+      </c>
+      <c r="B2" s="39" t="s">
+        <v>57</v>
+      </c>
+      <c r="C2" s="40" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="18" x14ac:dyDescent="0.2">
+      <c r="A3" s="39" t="s">
+        <v>58</v>
+      </c>
+      <c r="B3" s="39" t="s">
+        <v>59</v>
+      </c>
+      <c r="C3" s="39" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="18" x14ac:dyDescent="0.2">
+      <c r="A4" s="41" t="s">
         <v>61</v>
       </c>
-      <c r="B2" s="40" t="s">
+      <c r="B4" s="41" t="s">
+        <v>69</v>
+      </c>
+      <c r="C4" s="41" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="18" x14ac:dyDescent="0.2">
+      <c r="A5" s="41" t="s">
+        <v>64</v>
+      </c>
+      <c r="B5" s="41" t="s">
         <v>62</v>
       </c>
-      <c r="C2" s="41" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="18" x14ac:dyDescent="0.2">
-      <c r="A3" s="40" t="s">
-        <v>63</v>
-      </c>
-      <c r="B3" s="40" t="s">
-        <v>64</v>
-      </c>
-      <c r="C3" s="40" t="s">
+      <c r="C5" s="41" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="18" x14ac:dyDescent="0.2">
-      <c r="A4" s="42" t="s">
+    <row r="6" spans="1:3" ht="18" x14ac:dyDescent="0.2">
+      <c r="A6" s="41" t="s">
         <v>66</v>
       </c>
-      <c r="B4" s="42" t="s">
+      <c r="B6" s="41" t="s">
+        <v>62</v>
+      </c>
+      <c r="C6" s="41" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="18" x14ac:dyDescent="0.2">
+      <c r="A7" s="41" t="s">
+        <v>68</v>
+      </c>
+      <c r="B7" s="41" t="s">
+        <v>69</v>
+      </c>
+      <c r="C7" s="41" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="18" x14ac:dyDescent="0.2">
+      <c r="A8" s="41" t="s">
+        <v>71</v>
+      </c>
+      <c r="B8" s="41" t="s">
+        <v>69</v>
+      </c>
+      <c r="C8" s="41" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="19" x14ac:dyDescent="0.2">
+      <c r="A9" s="39" t="s">
+        <v>73</v>
+      </c>
+      <c r="B9" s="39" t="s">
         <v>74</v>
       </c>
-      <c r="C4" s="42" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="18" x14ac:dyDescent="0.2">
-      <c r="A5" s="42" t="s">
+      <c r="C9" s="42" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="18" x14ac:dyDescent="0.2">
+      <c r="A10" s="39" t="s">
+        <v>76</v>
+      </c>
+      <c r="B10" s="39">
+        <v>5000</v>
+      </c>
+      <c r="C10" s="39" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="19" x14ac:dyDescent="0.2">
+      <c r="A11" s="39" t="s">
+        <v>78</v>
+      </c>
+      <c r="B11" s="39">
+        <v>0.05</v>
+      </c>
+      <c r="C11" s="42" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="18" x14ac:dyDescent="0.2">
+      <c r="A12" s="43" t="s">
+        <v>80</v>
+      </c>
+      <c r="B12" s="43" t="s">
         <v>69</v>
       </c>
-      <c r="B5" s="42" t="s">
-        <v>67</v>
-      </c>
-      <c r="C5" s="42" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="18" x14ac:dyDescent="0.2">
-      <c r="A6" s="42" t="s">
-        <v>71</v>
-      </c>
-      <c r="B6" s="42" t="s">
-        <v>67</v>
-      </c>
-      <c r="C6" s="42" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="18" x14ac:dyDescent="0.2">
-      <c r="A7" s="42" t="s">
-        <v>73</v>
-      </c>
-      <c r="B7" s="42" t="s">
-        <v>74</v>
-      </c>
-      <c r="C7" s="42" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" ht="18" x14ac:dyDescent="0.2">
-      <c r="A8" s="42" t="s">
-        <v>76</v>
-      </c>
-      <c r="B8" s="42" t="s">
-        <v>74</v>
-      </c>
-      <c r="C8" s="42" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" ht="19" x14ac:dyDescent="0.2">
-      <c r="A9" s="40" t="s">
-        <v>78</v>
-      </c>
-      <c r="B9" s="40" t="s">
-        <v>79</v>
-      </c>
-      <c r="C9" s="43" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" ht="18" x14ac:dyDescent="0.2">
-      <c r="A10" s="40" t="s">
+      <c r="C12" s="43" t="s">
         <v>81</v>
-      </c>
-      <c r="B10" s="40">
-        <v>5000</v>
-      </c>
-      <c r="C10" s="40" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" ht="19" x14ac:dyDescent="0.2">
-      <c r="A11" s="40" t="s">
-        <v>83</v>
-      </c>
-      <c r="B11" s="40">
-        <v>0.05</v>
-      </c>
-      <c r="C11" s="43" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" ht="18" x14ac:dyDescent="0.2">
-      <c r="A12" s="44" t="s">
-        <v>85</v>
-      </c>
-      <c r="B12" s="44" t="s">
-        <v>74</v>
-      </c>
-      <c r="C12" s="44" t="s">
-        <v>86</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="B1:B1048576">
-    <cfRule type="containsText" dxfId="3" priority="1" operator="containsText" text="no">
+    <cfRule type="containsText" dxfId="5" priority="1" operator="containsText" text="no">
       <formula>NOT(ISERROR(SEARCH("no",B1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="2" priority="2" operator="containsText" text="yes">
+    <cfRule type="containsText" dxfId="4" priority="2" operator="containsText" text="yes">
       <formula>NOT(ISERROR(SEARCH("yes",B1)))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
move the statistical part in a new sub-function and update template excels
</commit_message>
<xml_diff>
--- a/template_files/template_parameters_analysis.xlsx
+++ b/template_files/template_parameters_analysis.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/u0112736/Documents/MATLAB/net/template_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00613AA6-8E46-6849-A1E4-9A927CB003AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94FB47D1-B650-0A4F-A9B9-BFD211EF1235}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10060" yWindow="760" windowWidth="20180" windowHeight="16100" activeTab="1" xr2:uid="{6EC9E106-9E35-B247-8D86-0F73FA459190}"/>
+    <workbookView xWindow="10060" yWindow="760" windowWidth="20180" windowHeight="16100" activeTab="2" xr2:uid="{6EC9E106-9E35-B247-8D86-0F73FA459190}"/>
   </bookViews>
   <sheets>
     <sheet name="activity_analysis" sheetId="1" r:id="rId1"/>
@@ -247,9 +247,6 @@
     <t>all</t>
   </si>
   <si>
-    <t xml:space="preserve"> 'all', 'none' or list of dataset separated by spaces</t>
-  </si>
-  <si>
     <t>stats.demean</t>
   </si>
   <si>
@@ -329,6 +326,9 @@
   </si>
   <si>
     <t>template_10_July</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'all', 'none', list of dataset separated by commas or first_dataset:last_dataset. Do not use spaces</t>
   </si>
 </sst>
 </file>
@@ -727,21 +727,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="10">
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF00B050"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
+  <dxfs count="8">
     <dxf>
       <font>
         <b/>
@@ -1167,7 +1153,7 @@
         <v>8</v>
       </c>
       <c r="B4" s="15" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C4" s="10" t="s">
         <v>9</v>
@@ -1211,7 +1197,7 @@
         <v>15</v>
       </c>
       <c r="B8" s="15" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C8" s="16" t="s">
         <v>16</v>
@@ -1244,7 +1230,7 @@
         <v>19</v>
       </c>
       <c r="B11" s="34" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C11" s="22" t="s">
         <v>9</v>
@@ -1288,26 +1274,26 @@
         <v>23</v>
       </c>
       <c r="B15" s="27" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C15" s="28" t="s">
         <v>16</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B12:B1048576 B1:B10">
-    <cfRule type="cellIs" dxfId="9" priority="5" operator="equal">
+  <conditionalFormatting sqref="B1:B10 B12:B1048576">
+    <cfRule type="cellIs" dxfId="7" priority="5" operator="equal">
       <formula>"off"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="6" operator="equal">
       <formula>"on"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B11">
-    <cfRule type="beginsWith" dxfId="3" priority="3" operator="beginsWith" text="off">
+    <cfRule type="beginsWith" dxfId="5" priority="3" operator="beginsWith" text="off">
       <formula>LEFT(B11,LEN("off"))="off"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="2" priority="4" operator="beginsWith" text="on">
+    <cfRule type="beginsWith" dxfId="4" priority="4" operator="beginsWith" text="on">
       <formula>LEFT(B11,LEN("on"))="on"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1319,7 +1305,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B89B74C7-BC73-5F44-99BC-879A3B054F87}">
   <dimension ref="A1:C20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
@@ -1443,10 +1429,10 @@
     </row>
     <row r="11" spans="1:3" ht="19" x14ac:dyDescent="0.2">
       <c r="A11" s="11" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B11" s="15" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C11" s="16" t="s">
         <v>16</v>
@@ -1534,7 +1520,7 @@
         <v>55</v>
       </c>
       <c r="B19" s="34" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C19" s="22" t="s">
         <v>9</v>
@@ -1542,21 +1528,21 @@
     </row>
     <row r="20" spans="1:3" ht="19" x14ac:dyDescent="0.2">
       <c r="A20" s="35" t="s">
+        <v>82</v>
+      </c>
+      <c r="B20" s="36" t="s">
+        <v>86</v>
+      </c>
+      <c r="C20" s="37" t="s">
         <v>83</v>
-      </c>
-      <c r="B20" s="36" t="s">
-        <v>87</v>
-      </c>
-      <c r="C20" s="37" t="s">
-        <v>84</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="B1:B1048576">
-    <cfRule type="beginsWith" dxfId="7" priority="1" operator="beginsWith" text="off">
+    <cfRule type="beginsWith" dxfId="3" priority="1" operator="beginsWith" text="off">
       <formula>LEFT(B1,LEN("off"))="off"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="6" priority="2" operator="beginsWith" text="on">
+    <cfRule type="beginsWith" dxfId="2" priority="2" operator="beginsWith" text="on">
       <formula>LEFT(B1,LEN("on"))="on"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1568,8 +1554,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A225D7CE-8777-D54B-A402-94CEC95943B4}">
   <dimension ref="A1:C12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="25" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1598,7 +1584,7 @@
         <v>57</v>
       </c>
       <c r="C2" s="40" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="18" x14ac:dyDescent="0.2">
@@ -1609,114 +1595,114 @@
         <v>59</v>
       </c>
       <c r="C3" s="39" t="s">
-        <v>60</v>
+        <v>87</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="18" x14ac:dyDescent="0.2">
       <c r="A4" s="41" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B4" s="41" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C4" s="41" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="18" x14ac:dyDescent="0.2">
       <c r="A5" s="41" t="s">
+        <v>63</v>
+      </c>
+      <c r="B5" s="41" t="s">
+        <v>61</v>
+      </c>
+      <c r="C5" s="41" t="s">
         <v>64</v>
-      </c>
-      <c r="B5" s="41" t="s">
-        <v>62</v>
-      </c>
-      <c r="C5" s="41" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="18" x14ac:dyDescent="0.2">
       <c r="A6" s="41" t="s">
+        <v>65</v>
+      </c>
+      <c r="B6" s="41" t="s">
+        <v>61</v>
+      </c>
+      <c r="C6" s="41" t="s">
         <v>66</v>
-      </c>
-      <c r="B6" s="41" t="s">
-        <v>62</v>
-      </c>
-      <c r="C6" s="41" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="18" x14ac:dyDescent="0.2">
       <c r="A7" s="41" t="s">
+        <v>67</v>
+      </c>
+      <c r="B7" s="41" t="s">
         <v>68</v>
       </c>
-      <c r="B7" s="41" t="s">
+      <c r="C7" s="41" t="s">
         <v>69</v>
-      </c>
-      <c r="C7" s="41" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="18" x14ac:dyDescent="0.2">
       <c r="A8" s="41" t="s">
+        <v>70</v>
+      </c>
+      <c r="B8" s="41" t="s">
+        <v>68</v>
+      </c>
+      <c r="C8" s="41" t="s">
         <v>71</v>
-      </c>
-      <c r="B8" s="41" t="s">
-        <v>69</v>
-      </c>
-      <c r="C8" s="41" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="19" x14ac:dyDescent="0.2">
       <c r="A9" s="39" t="s">
+        <v>72</v>
+      </c>
+      <c r="B9" s="39" t="s">
         <v>73</v>
       </c>
-      <c r="B9" s="39" t="s">
+      <c r="C9" s="42" t="s">
         <v>74</v>
-      </c>
-      <c r="C9" s="42" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="18" x14ac:dyDescent="0.2">
       <c r="A10" s="39" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B10" s="39">
         <v>5000</v>
       </c>
       <c r="C10" s="39" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="19" x14ac:dyDescent="0.2">
       <c r="A11" s="39" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B11" s="39">
         <v>0.05</v>
       </c>
       <c r="C11" s="42" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="18" x14ac:dyDescent="0.2">
       <c r="A12" s="43" t="s">
+        <v>79</v>
+      </c>
+      <c r="B12" s="43" t="s">
+        <v>68</v>
+      </c>
+      <c r="C12" s="43" t="s">
         <v>80</v>
-      </c>
-      <c r="B12" s="43" t="s">
-        <v>69</v>
-      </c>
-      <c r="C12" s="43" t="s">
-        <v>81</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="B1:B1048576">
-    <cfRule type="containsText" dxfId="5" priority="1" operator="containsText" text="no">
+    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="no">
       <formula>NOT(ISERROR(SEARCH("no",B1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="4" priority="2" operator="containsText" text="yes">
+    <cfRule type="containsText" dxfId="0" priority="2" operator="containsText" text="yes">
       <formula>NOT(ISERROR(SEARCH("yes",B1)))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
final excel for test data
</commit_message>
<xml_diff>
--- a/template_files/template_parameters_analysis.xlsx
+++ b/template_files/template_parameters_analysis.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/u0112736/Documents/MATLAB/net/template_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94FB47D1-B650-0A4F-A9B9-BFD211EF1235}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{308245B2-6869-624C-BD27-765D93C25F06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10060" yWindow="760" windowWidth="20180" windowHeight="16100" activeTab="2" xr2:uid="{6EC9E106-9E35-B247-8D86-0F73FA459190}"/>
+    <workbookView xWindow="10060" yWindow="760" windowWidth="20180" windowHeight="16100" activeTab="1" xr2:uid="{6EC9E106-9E35-B247-8D86-0F73FA459190}"/>
   </bookViews>
   <sheets>
     <sheet name="activity_analysis" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="88">
   <si>
     <t>parameters_name</t>
   </si>
@@ -247,6 +247,9 @@
     <t>all</t>
   </si>
   <si>
+    <t xml:space="preserve"> 'all', 'none' or list of dataset separated by spaces</t>
+  </si>
+  <si>
     <t>stats.demean</t>
   </si>
   <si>
@@ -325,10 +328,7 @@
     <t>template_seeds</t>
   </si>
   <si>
-    <t>template_10_July</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 'all', 'none', list of dataset separated by commas or first_dataset:last_dataset. Do not use spaces</t>
+    <t>template_triggers</t>
   </si>
 </sst>
 </file>
@@ -592,7 +592,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -620,6 +620,9 @@
     </xf>
     <xf numFmtId="49" fontId="2" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -727,21 +730,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="8">
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF00B050"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
+  <dxfs count="6">
     <dxf>
       <font>
         <b/>
@@ -1104,7 +1093,7 @@
   <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1131,7 +1120,7 @@
         <v>3</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>5</v>
@@ -1142,7 +1131,7 @@
         <v>6</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C3" s="8" t="s">
         <v>5</v>
@@ -1152,10 +1141,10 @@
       <c r="A4" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="15" t="s">
-        <v>85</v>
-      </c>
-      <c r="C4" s="10" t="s">
+      <c r="B4" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="C4" s="11" t="s">
         <v>9</v>
       </c>
     </row>
@@ -1171,130 +1160,122 @@
       </c>
     </row>
     <row r="6" spans="1:3" ht="18" x14ac:dyDescent="0.2">
-      <c r="A6" s="11" t="s">
+      <c r="A6" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="12">
+      <c r="B6" s="13">
         <v>1</v>
       </c>
-      <c r="C6" s="13" t="s">
+      <c r="C6" s="14" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="18" x14ac:dyDescent="0.2">
-      <c r="A7" s="11" t="s">
+      <c r="A7" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="12">
+      <c r="B7" s="13">
         <v>80</v>
       </c>
-      <c r="C7" s="13" t="s">
+      <c r="C7" s="14" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="19" x14ac:dyDescent="0.2">
-      <c r="A8" s="14" t="s">
+      <c r="A8" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="B8" s="15" t="s">
+      <c r="B8" s="16" t="s">
+        <v>87</v>
+      </c>
+      <c r="C8" s="17" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="18" x14ac:dyDescent="0.2">
+      <c r="A9" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" s="20" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="18" x14ac:dyDescent="0.2">
+      <c r="A10" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10" s="20" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="19" x14ac:dyDescent="0.2">
+      <c r="A11" s="21" t="s">
+        <v>19</v>
+      </c>
+      <c r="B11" s="22" t="s">
         <v>86</v>
       </c>
-      <c r="C8" s="16" t="s">
+      <c r="C11" s="23" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="18" x14ac:dyDescent="0.2">
+      <c r="A12" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="B12" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="C12" s="20" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="18" x14ac:dyDescent="0.2">
+      <c r="A13" s="24" t="s">
+        <v>21</v>
+      </c>
+      <c r="B13" s="25">
+        <v>1</v>
+      </c>
+      <c r="C13" s="26" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="18" x14ac:dyDescent="0.2">
+      <c r="A14" s="24" t="s">
+        <v>22</v>
+      </c>
+      <c r="B14" s="25">
+        <v>80</v>
+      </c>
+      <c r="C14" s="26" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="19" x14ac:dyDescent="0.2">
+      <c r="A15" s="27" t="s">
+        <v>23</v>
+      </c>
+      <c r="B15" s="28" t="s">
+        <v>87</v>
+      </c>
+      <c r="C15" s="29" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="18" x14ac:dyDescent="0.2">
-      <c r="A9" s="17" t="s">
-        <v>17</v>
-      </c>
-      <c r="B9" s="18" t="s">
-        <v>7</v>
-      </c>
-      <c r="C9" s="19" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" ht="18" x14ac:dyDescent="0.2">
-      <c r="A10" s="17" t="s">
-        <v>18</v>
-      </c>
-      <c r="B10" s="18" t="s">
-        <v>7</v>
-      </c>
-      <c r="C10" s="19" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" ht="19" x14ac:dyDescent="0.2">
-      <c r="A11" s="20" t="s">
-        <v>19</v>
-      </c>
-      <c r="B11" s="34" t="s">
-        <v>85</v>
-      </c>
-      <c r="C11" s="22" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" ht="18" x14ac:dyDescent="0.2">
-      <c r="A12" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="B12" s="18" t="s">
-        <v>7</v>
-      </c>
-      <c r="C12" s="19" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" ht="18" x14ac:dyDescent="0.2">
-      <c r="A13" s="23" t="s">
-        <v>21</v>
-      </c>
-      <c r="B13" s="24">
-        <v>1</v>
-      </c>
-      <c r="C13" s="25" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" ht="18" x14ac:dyDescent="0.2">
-      <c r="A14" s="23" t="s">
-        <v>22</v>
-      </c>
-      <c r="B14" s="24">
-        <v>80</v>
-      </c>
-      <c r="C14" s="25" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" ht="19" x14ac:dyDescent="0.2">
-      <c r="A15" s="26" t="s">
-        <v>23</v>
-      </c>
-      <c r="B15" s="27" t="s">
-        <v>86</v>
-      </c>
-      <c r="C15" s="28" t="s">
-        <v>16</v>
-      </c>
-    </row>
   </sheetData>
-  <conditionalFormatting sqref="B1:B10 B12:B1048576">
-    <cfRule type="cellIs" dxfId="7" priority="5" operator="equal">
+  <conditionalFormatting sqref="B1:B1048576">
+    <cfRule type="cellIs" dxfId="5" priority="1" operator="equal">
       <formula>"off"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="2" operator="equal">
       <formula>"on"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B11">
-    <cfRule type="beginsWith" dxfId="5" priority="3" operator="beginsWith" text="off">
-      <formula>LEFT(B11,LEN("off"))="off"</formula>
-    </cfRule>
-    <cfRule type="beginsWith" dxfId="4" priority="4" operator="beginsWith" text="on">
-      <formula>LEFT(B11,LEN("on"))="on"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1305,8 +1286,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B89B74C7-BC73-5F44-99BC-879A3B054F87}">
   <dimension ref="A1:C20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1318,13 +1299,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="18" x14ac:dyDescent="0.2">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="30" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="30" t="s">
+      <c r="C1" s="31" t="s">
         <v>2</v>
       </c>
     </row>
@@ -1340,201 +1321,197 @@
       </c>
     </row>
     <row r="3" spans="1:3" ht="18" x14ac:dyDescent="0.2">
-      <c r="A3" s="11" t="s">
+      <c r="A3" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="B3" s="12">
+      <c r="B3" s="13">
         <v>1</v>
       </c>
-      <c r="C3" s="13" t="s">
+      <c r="C3" s="14" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="18" x14ac:dyDescent="0.2">
-      <c r="A4" s="11" t="s">
+      <c r="A4" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="B4" s="12">
+      <c r="B4" s="13">
         <v>80</v>
       </c>
-      <c r="C4" s="13" t="s">
+      <c r="C4" s="14" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="18" x14ac:dyDescent="0.2">
-      <c r="A5" s="11" t="s">
+      <c r="A5" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="B5" s="12">
+      <c r="B5" s="13">
         <v>2</v>
       </c>
-      <c r="C5" s="13" t="s">
+      <c r="C5" s="14" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="18" x14ac:dyDescent="0.2">
-      <c r="A6" s="11" t="s">
+      <c r="A6" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="B6" s="12">
+      <c r="B6" s="13">
         <v>1</v>
       </c>
-      <c r="C6" s="13" t="s">
+      <c r="C6" s="14" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="18" x14ac:dyDescent="0.2">
-      <c r="A7" s="11" t="s">
+      <c r="A7" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="B7" s="12">
+      <c r="B7" s="13">
         <v>6</v>
       </c>
-      <c r="C7" s="13" t="s">
+      <c r="C7" s="14" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="18" x14ac:dyDescent="0.2">
-      <c r="A8" s="11" t="s">
+      <c r="A8" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="B8" s="12" t="s">
+      <c r="B8" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="C8" s="13" t="s">
+      <c r="C8" s="14" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="18" x14ac:dyDescent="0.2">
-      <c r="A9" s="11" t="s">
+      <c r="A9" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="B9" s="31" t="s">
+      <c r="B9" s="32" t="s">
         <v>38</v>
       </c>
-      <c r="C9" s="13" t="s">
+      <c r="C9" s="14" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="18" x14ac:dyDescent="0.2">
-      <c r="A10" s="11" t="s">
+      <c r="A10" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="B10" s="12" t="s">
+      <c r="B10" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="C10" s="13" t="s">
+      <c r="C10" s="14" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="19" x14ac:dyDescent="0.2">
-      <c r="A11" s="11" t="s">
-        <v>81</v>
-      </c>
-      <c r="B11" s="15" t="s">
+      <c r="A11" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="B11" s="16"/>
+      <c r="C11" s="17" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="18" x14ac:dyDescent="0.2">
+      <c r="A12" s="18" t="s">
+        <v>43</v>
+      </c>
+      <c r="B12" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="C12" s="20" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="18" x14ac:dyDescent="0.2">
+      <c r="A13" s="18" t="s">
+        <v>44</v>
+      </c>
+      <c r="B13" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="C13" s="20" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="18" x14ac:dyDescent="0.2">
+      <c r="A14" s="24" t="s">
+        <v>45</v>
+      </c>
+      <c r="B14" s="33">
+        <v>2</v>
+      </c>
+      <c r="C14" s="26" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="18" x14ac:dyDescent="0.2">
+      <c r="A15" s="24" t="s">
+        <v>46</v>
+      </c>
+      <c r="B15" s="33">
+        <v>1</v>
+      </c>
+      <c r="C15" s="26" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="19" x14ac:dyDescent="0.2">
+      <c r="A16" s="21" t="s">
+        <v>47</v>
+      </c>
+      <c r="B16" s="22" t="s">
+        <v>48</v>
+      </c>
+      <c r="C16" s="34" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="19" x14ac:dyDescent="0.2">
+      <c r="A17" s="21" t="s">
+        <v>50</v>
+      </c>
+      <c r="B17" s="22" t="s">
+        <v>51</v>
+      </c>
+      <c r="C17" s="23" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="19" x14ac:dyDescent="0.2">
+      <c r="A18" s="21" t="s">
+        <v>53</v>
+      </c>
+      <c r="B18" s="35">
+        <v>1000</v>
+      </c>
+      <c r="C18" s="23" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="19" x14ac:dyDescent="0.2">
+      <c r="A19" s="21" t="s">
+        <v>55</v>
+      </c>
+      <c r="B19" s="35" t="s">
         <v>86</v>
       </c>
-      <c r="C11" s="16" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" ht="18" x14ac:dyDescent="0.2">
-      <c r="A12" s="17" t="s">
-        <v>43</v>
-      </c>
-      <c r="B12" s="18" t="s">
-        <v>4</v>
-      </c>
-      <c r="C12" s="19" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" ht="18" x14ac:dyDescent="0.2">
-      <c r="A13" s="17" t="s">
-        <v>44</v>
-      </c>
-      <c r="B13" s="18" t="s">
-        <v>4</v>
-      </c>
-      <c r="C13" s="19" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" ht="18" x14ac:dyDescent="0.2">
-      <c r="A14" s="23" t="s">
-        <v>45</v>
-      </c>
-      <c r="B14" s="32">
-        <v>2</v>
-      </c>
-      <c r="C14" s="25" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" ht="18" x14ac:dyDescent="0.2">
-      <c r="A15" s="23" t="s">
-        <v>46</v>
-      </c>
-      <c r="B15" s="32">
-        <v>1</v>
-      </c>
-      <c r="C15" s="25" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" ht="19" x14ac:dyDescent="0.2">
-      <c r="A16" s="20" t="s">
-        <v>47</v>
-      </c>
-      <c r="B16" s="21" t="s">
-        <v>48</v>
-      </c>
-      <c r="C16" s="33" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" ht="19" x14ac:dyDescent="0.2">
-      <c r="A17" s="20" t="s">
-        <v>50</v>
-      </c>
-      <c r="B17" s="21" t="s">
-        <v>51</v>
-      </c>
-      <c r="C17" s="22" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" ht="19" x14ac:dyDescent="0.2">
-      <c r="A18" s="20" t="s">
-        <v>53</v>
-      </c>
-      <c r="B18" s="34">
-        <v>1000</v>
-      </c>
-      <c r="C18" s="22" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" ht="19" x14ac:dyDescent="0.2">
-      <c r="A19" s="20" t="s">
-        <v>55</v>
-      </c>
-      <c r="B19" s="34" t="s">
-        <v>85</v>
-      </c>
-      <c r="C19" s="22" t="s">
+      <c r="C19" s="23" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="19" x14ac:dyDescent="0.2">
-      <c r="A20" s="35" t="s">
-        <v>82</v>
-      </c>
-      <c r="B20" s="36" t="s">
-        <v>86</v>
-      </c>
-      <c r="C20" s="37" t="s">
+      <c r="A20" s="36" t="s">
         <v>83</v>
+      </c>
+      <c r="B20" s="37"/>
+      <c r="C20" s="38" t="s">
+        <v>84</v>
       </c>
     </row>
   </sheetData>
@@ -1554,8 +1531,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A225D7CE-8777-D54B-A402-94CEC95943B4}">
   <dimension ref="A1:C12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="25" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1566,135 +1543,135 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="18" x14ac:dyDescent="0.2">
-      <c r="A1" s="38" t="s">
+      <c r="A1" s="39" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="38" t="s">
+      <c r="B1" s="39" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="38" t="s">
+      <c r="C1" s="39" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="18" x14ac:dyDescent="0.2">
-      <c r="A2" s="39" t="s">
+      <c r="A2" s="40" t="s">
         <v>56</v>
       </c>
-      <c r="B2" s="39" t="s">
+      <c r="B2" s="40" t="s">
         <v>57</v>
       </c>
-      <c r="C2" s="40" t="s">
-        <v>84</v>
+      <c r="C2" s="41" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="18" x14ac:dyDescent="0.2">
-      <c r="A3" s="39" t="s">
+      <c r="A3" s="40" t="s">
         <v>58</v>
       </c>
-      <c r="B3" s="39" t="s">
+      <c r="B3" s="40" t="s">
         <v>59</v>
       </c>
-      <c r="C3" s="39" t="s">
-        <v>87</v>
+      <c r="C3" s="40" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="18" x14ac:dyDescent="0.2">
-      <c r="A4" s="41" t="s">
-        <v>60</v>
-      </c>
-      <c r="B4" s="41" t="s">
+      <c r="A4" s="42" t="s">
+        <v>61</v>
+      </c>
+      <c r="B4" s="42" t="s">
+        <v>69</v>
+      </c>
+      <c r="C4" s="42" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="18" x14ac:dyDescent="0.2">
+      <c r="A5" s="42" t="s">
+        <v>64</v>
+      </c>
+      <c r="B5" s="42" t="s">
+        <v>62</v>
+      </c>
+      <c r="C5" s="42" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="18" x14ac:dyDescent="0.2">
+      <c r="A6" s="42" t="s">
+        <v>66</v>
+      </c>
+      <c r="B6" s="42" t="s">
+        <v>62</v>
+      </c>
+      <c r="C6" s="42" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="18" x14ac:dyDescent="0.2">
+      <c r="A7" s="42" t="s">
         <v>68</v>
       </c>
-      <c r="C4" s="41" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="18" x14ac:dyDescent="0.2">
-      <c r="A5" s="41" t="s">
-        <v>63</v>
-      </c>
-      <c r="B5" s="41" t="s">
-        <v>61</v>
-      </c>
-      <c r="C5" s="41" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="18" x14ac:dyDescent="0.2">
-      <c r="A6" s="41" t="s">
-        <v>65</v>
-      </c>
-      <c r="B6" s="41" t="s">
-        <v>61</v>
-      </c>
-      <c r="C6" s="41" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="18" x14ac:dyDescent="0.2">
-      <c r="A7" s="41" t="s">
-        <v>67</v>
-      </c>
-      <c r="B7" s="41" t="s">
-        <v>68</v>
-      </c>
-      <c r="C7" s="41" t="s">
+      <c r="B7" s="42" t="s">
         <v>69</v>
       </c>
+      <c r="C7" s="42" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="8" spans="1:3" ht="18" x14ac:dyDescent="0.2">
-      <c r="A8" s="41" t="s">
-        <v>70</v>
-      </c>
-      <c r="B8" s="41" t="s">
-        <v>68</v>
-      </c>
-      <c r="C8" s="41" t="s">
+      <c r="A8" s="42" t="s">
         <v>71</v>
       </c>
+      <c r="B8" s="42" t="s">
+        <v>69</v>
+      </c>
+      <c r="C8" s="42" t="s">
+        <v>72</v>
+      </c>
     </row>
     <row r="9" spans="1:3" ht="19" x14ac:dyDescent="0.2">
-      <c r="A9" s="39" t="s">
-        <v>72</v>
-      </c>
-      <c r="B9" s="39" t="s">
+      <c r="A9" s="40" t="s">
         <v>73</v>
       </c>
-      <c r="C9" s="42" t="s">
+      <c r="B9" s="40" t="s">
         <v>74</v>
       </c>
+      <c r="C9" s="43" t="s">
+        <v>75</v>
+      </c>
     </row>
     <row r="10" spans="1:3" ht="18" x14ac:dyDescent="0.2">
-      <c r="A10" s="39" t="s">
-        <v>75</v>
-      </c>
-      <c r="B10" s="39">
+      <c r="A10" s="40" t="s">
+        <v>76</v>
+      </c>
+      <c r="B10" s="40">
         <v>5000</v>
       </c>
-      <c r="C10" s="39" t="s">
-        <v>76</v>
+      <c r="C10" s="40" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="19" x14ac:dyDescent="0.2">
-      <c r="A11" s="39" t="s">
-        <v>77</v>
-      </c>
-      <c r="B11" s="39">
+      <c r="A11" s="40" t="s">
+        <v>78</v>
+      </c>
+      <c r="B11" s="40">
         <v>0.05</v>
       </c>
-      <c r="C11" s="42" t="s">
-        <v>78</v>
+      <c r="C11" s="43" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="18" x14ac:dyDescent="0.2">
-      <c r="A12" s="43" t="s">
-        <v>79</v>
-      </c>
-      <c r="B12" s="43" t="s">
-        <v>68</v>
-      </c>
-      <c r="C12" s="43" t="s">
+      <c r="A12" s="44" t="s">
         <v>80</v>
+      </c>
+      <c r="B12" s="44" t="s">
+        <v>69</v>
+      </c>
+      <c r="C12" s="44" t="s">
+        <v>81</v>
       </c>
     </row>
   </sheetData>

</xml_diff>